<commit_message>
Finalização do Doc do projeto
</commit_message>
<xml_diff>
--- a/doc/em-andamento/Planilha-de-riscos-Strongberry.xlsx
+++ b/doc/em-andamento/Planilha-de-riscos-Strongberry.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roberta\Desktop\workspace\Faculdade\Bandtec\Projeto Sprint2\strongberry2\StrongBerry\Documentação\em-andamento\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roberta\Desktop\workspace\Faculdade\Bandtec\StrongBerry\doc\em-andamento\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85240525-EEAC-48FE-A018-E77C0FFDBE5A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9539C66-6F86-4470-B7F9-53AE35A2FF48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4FE799BE-7C5F-4A5D-AA14-D10458B4BB43}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
   <si>
     <t>ID</t>
   </si>
@@ -162,6 +162,15 @@
   </si>
   <si>
     <t>R5</t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>Gestão de tempo em relação ao projeto individual e o projeto em grupo</t>
+  </si>
+  <si>
+    <t>Organizar o tempo em relação aos dois porjetos para todos os integrantes.</t>
   </si>
 </sst>
 </file>
@@ -616,7 +625,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB85EF7C-7F67-4C50-BDBB-DA5E702B3666}">
-  <dimension ref="A1:L35"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="I10" sqref="I10"/>
@@ -627,17 +636,15 @@
     <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.42578125" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="75.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="20.7109375" customWidth="1"/>
+    <col min="7" max="7" width="114" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="21.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="63" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="63" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -659,14 +666,8 @@
       <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-    </row>
-    <row r="2" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>34</v>
       </c>
@@ -688,20 +689,8 @@
       <c r="G2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="9">
-        <v>3</v>
-      </c>
-      <c r="K2" s="10">
-        <v>6</v>
-      </c>
-      <c r="L2" s="10">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>35</v>
       </c>
@@ -723,20 +712,8 @@
       <c r="G3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="J3" s="11">
-        <v>2</v>
-      </c>
-      <c r="K3" s="9">
-        <v>4</v>
-      </c>
-      <c r="L3" s="10">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>36</v>
       </c>
@@ -758,20 +735,8 @@
       <c r="G4" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="J4" s="11">
-        <v>1</v>
-      </c>
-      <c r="K4" s="11">
-        <v>2</v>
-      </c>
-      <c r="L4" s="9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>37</v>
       </c>
@@ -793,18 +758,8 @@
       <c r="G5" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="K5" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="L5" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>38</v>
       </c>
@@ -826,81 +781,155 @@
       <c r="G6" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8" t="s">
+    </row>
+    <row r="7" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="5">
+        <v>2</v>
+      </c>
+      <c r="D7" s="5">
+        <v>3</v>
+      </c>
+      <c r="E7" s="5">
+        <v>6</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+    </row>
+    <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>2211043</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="9">
+        <v>3</v>
+      </c>
+      <c r="E10" s="10">
+        <v>6</v>
+      </c>
+      <c r="F10" s="10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>2211028</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="11">
+        <v>2</v>
+      </c>
+      <c r="E11" s="9">
+        <v>4</v>
+      </c>
+      <c r="F11" s="10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>2211011</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="11">
+        <v>1</v>
+      </c>
+      <c r="E12" s="11">
+        <v>2</v>
+      </c>
+      <c r="F12" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>2211057</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>2211038</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="L6" s="8"/>
-    </row>
-    <row r="7" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>2211043</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
-        <v>2211028</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <v>2211011</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
-        <v>2211057</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
-        <v>2211038</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="F14" s="8"/>
+    </row>
+    <row r="15" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>